<commit_message>
increased sleep time in duplicateGstin create
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
   <si>
     <t xml:space="preserve">userId</t>
   </si>
@@ -214,13 +214,16 @@
     <t xml:space="preserve">33qiwuj323451z5</t>
   </si>
   <si>
+    <t xml:space="preserve">EOEK/12-1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mad mans systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33qpwuj323451z5</t>
+  </si>
+  <si>
     <t xml:space="preserve">YEHE82727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mad mans systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33qpwuj323451z5</t>
   </si>
 </sst>
 </file>
@@ -340,7 +343,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -363,7 +366,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -613,7 +616,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -812,10 +815,10 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -946,7 +949,7 @@
         <v>2726287</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
common changes made in tradingbase utility class in trunk1.0
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -208,16 +208,16 @@
     <t xml:space="preserve">vendorType</t>
   </si>
   <si>
-    <t xml:space="preserve">Genesys cad systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33qiwuj323451z5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EOEK/12-1019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mad mans systems</t>
+    <t xml:space="preserve">mashsy cad systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33qiquj323451z5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YEH-202/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iekenu mans systems</t>
   </si>
   <si>
     <t xml:space="preserve">33qpwuj323451z5</t>
@@ -343,7 +343,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -366,7 +366,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -616,7 +616,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -818,7 +818,10 @@
       <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="11.64"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
create customer F1 button added instead of webelement click
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="createCustomerDataFull" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
   <si>
     <t xml:space="preserve">userId</t>
   </si>
@@ -184,19 +184,16 @@
     <t xml:space="preserve">manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">UE/121-H1019</t>
+    <t xml:space="preserve">UE121H1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reg cust4</t>
   </si>
   <si>
     <t xml:space="preserve">33hbnwy223451z5</t>
   </si>
   <si>
     <t xml:space="preserve">theni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IEE8738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reg cust4</t>
   </si>
   <si>
     <t xml:space="preserve">IEKE0928</t>
@@ -343,7 +340,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -366,7 +363,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -610,13 +607,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -716,86 +713,44 @@
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>2367654314</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>875489</v>
+        <v>986587</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>2367654314</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>986587</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Pass@1234"/>
     <hyperlink ref="B3" r:id="rId2" display="Pass@1234"/>
-    <hyperlink ref="B4" r:id="rId3" display="Pass@1234"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -814,11 +769,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="11.64"/>
   </cols>
@@ -834,13 +789,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -878,10 +833,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>28</v>
@@ -908,7 +863,7 @@
         <v>2726287</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,10 +877,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>28</v>
@@ -952,7 +907,7 @@
         <v>2726287</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st commit for github webjook
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="createCustomerDataFull" sheetId="1" state="visible" r:id="rId2"/>
@@ -340,7 +340,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -363,7 +363,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -609,11 +609,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -769,14 +769,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="11.64"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
webhook change- customer excel data change
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="createCustomerDataFull" sheetId="1" state="visible" r:id="rId2"/>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">theni</t>
   </si>
   <si>
-    <t xml:space="preserve">IEKE0928</t>
+    <t xml:space="preserve">IEKE0/928</t>
   </si>
   <si>
     <t xml:space="preserve">vendorName</t>
@@ -340,7 +340,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -363,7 +363,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -609,11 +609,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -769,11 +769,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
excel data change to pass cases sheet name changed
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="createCustomerDataFull" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="createCustomerData" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="customer" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="vendor" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">theni</t>
   </si>
   <si>
-    <t xml:space="preserve">IEKE0/92812</t>
+    <t xml:space="preserve">IEKE092812</t>
   </si>
   <si>
     <t xml:space="preserve">vendorName</t>
@@ -340,7 +340,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -363,7 +363,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -609,11 +609,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -769,11 +769,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
c/p for sales invoice add changes
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="createCustomerDataFull" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="createCustomerData" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="customer" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="vendor" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="salesInvoice" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
   <si>
     <t xml:space="preserve">userId</t>
   </si>
@@ -221,6 +222,57 @@
   </si>
   <si>
     <t xml:space="preserve">YEHE82727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sampleId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paymentMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inv-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tirupur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net banking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zas Black Cardamom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zas BlackGram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inv-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zachary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gowtham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sbi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zas DryChilli</t>
   </si>
 </sst>
 </file>
@@ -337,10 +389,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:G3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -360,10 +412,10 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:G3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -610,10 +662,10 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+      <selection pane="topLeft" activeCell="N7" activeCellId="1" sqref="B3:G3 N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -769,11 +821,11 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="B3:G3 K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -920,4 +972,161 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="Pass@1234"/>
+    <hyperlink ref="C3" r:id="rId2" display="Pass@1234"/>
+    <hyperlink ref="C4" r:id="rId3" display="Pass@1234"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
xml sales invoice added commit 2.0
</commit_message>
<xml_diff>
--- a/erp-trading/testDataExternalFiles/LoginData.xlsx
+++ b/erp-trading/testDataExternalFiles/LoginData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="createCustomerDataFull" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
   <si>
     <t xml:space="preserve">userId</t>
   </si>
@@ -188,18 +188,6 @@
     <t xml:space="preserve">UE121H1019</t>
   </si>
   <si>
-    <t xml:space="preserve">reg cust4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33hbnwy223451z5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">theni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IEKE092812</t>
-  </si>
-  <si>
     <t xml:space="preserve">vendorName</t>
   </si>
   <si>
@@ -213,15 +201,6 @@
   </si>
   <si>
     <t xml:space="preserve">YEH20221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iekenu mans systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33qpwuj323451z5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YEHE82727</t>
   </si>
   <si>
     <t xml:space="preserve">sampleId</t>
@@ -389,10 +368,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:G3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -412,10 +391,10 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:G3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -659,13 +638,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="1" sqref="B3:G3 N7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="11.84"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -755,54 +737,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>2367654314</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>986587</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Pass@1234"/>
-    <hyperlink ref="B3" r:id="rId2" display="Pass@1234"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -819,13 +756,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="B3:G3 K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ALV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="11.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -838,13 +778,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -882,10 +822,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>28</v>
@@ -912,57 +852,12 @@
         <v>2726287</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>2546543425</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>2726287</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Pass@1234"/>
-    <hyperlink ref="B3" r:id="rId2" display="Pass@1234"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -981,15 +876,15 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1004,24 +899,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
@@ -1033,16 +928,16 @@
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>17</v>
@@ -1053,7 +948,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -1065,16 +960,16 @@
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>5</v>
@@ -1085,7 +980,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -1097,16 +992,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>25</v>

</xml_diff>